<commit_message>
Added 2 more test cases in input xl
</commit_message>
<xml_diff>
--- a/PythonWorkingScripts_InputData/Assessment/Audiotranscript/input_audio_transcript_cefr.xlsx
+++ b/PythonWorkingScripts_InputData/Assessment/Audiotranscript/input_audio_transcript_cefr.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="58">
   <si>
     <t xml:space="preserve">Test Cases</t>
   </si>
@@ -224,6 +224,15 @@
   </si>
   <si>
     <t xml:space="preserve">C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not answered candidate evaluated by spontaneous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not answered candidate evaluated by RAP</t>
   </si>
 </sst>
 </file>
@@ -306,13 +315,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -328,6 +341,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -523,189 +540,191 @@
   <dimension ref="A1:AO1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="43.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="4" style="1" width="12.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="17" style="2" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="12.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="1" width="12.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="31" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="4" t="s">
         <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AK1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AL1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AM1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AN1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AO1" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="4" t="n">
+      <c r="H2" s="5" t="n">
         <v>72.73</v>
       </c>
-      <c r="I2" s="4" t="n">
+      <c r="I2" s="5" t="n">
         <v>54.55</v>
       </c>
-      <c r="J2" s="4" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="K2" s="4" t="n">
+      <c r="J2" s="5" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="K2" s="5" t="n">
         <v>54.55</v>
       </c>
-      <c r="L2" s="4" t="n">
+      <c r="L2" s="5" t="n">
         <v>54.55</v>
       </c>
-      <c r="M2" s="4" t="n">
+      <c r="M2" s="5" t="n">
         <v>54.55</v>
       </c>
-      <c r="N2" s="3" t="n">
+      <c r="N2" s="4" t="n">
         <v>20609</v>
       </c>
-      <c r="O2" s="3" t="n">
+      <c r="O2" s="4" t="n">
         <v>3764377</v>
       </c>
       <c r="P2" s="1" t="n">
@@ -788,49 +807,49 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="3" t="n">
+      <c r="F3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="4" t="n">
         <v>54.55</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="3" t="n">
+      <c r="J3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="4" t="n">
         <v>54.55</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" s="3" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="N3" s="3" t="n">
+      <c r="L3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="4" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="N3" s="4" t="n">
         <v>20611</v>
       </c>
-      <c r="O3" s="5" t="n">
+      <c r="O3" s="6" t="n">
         <v>3764363</v>
       </c>
       <c r="P3" s="1" t="n">
@@ -913,49 +932,49 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="4" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="I4" s="4" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="J4" s="4" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="K4" s="4" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="L4" s="4" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="M4" s="4" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="N4" s="3" t="n">
+      <c r="B4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="N4" s="4" t="n">
         <v>20609</v>
       </c>
-      <c r="O4" s="5" t="n">
+      <c r="O4" s="6" t="n">
         <v>3764359</v>
       </c>
       <c r="P4" s="1" t="n">
@@ -1038,49 +1057,49 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="B5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="3" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="3" t="n">
+      <c r="H5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="4" t="n">
         <v>54.55</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="3" t="n">
+      <c r="L5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="4" t="n">
         <v>63.64</v>
       </c>
-      <c r="N5" s="3" t="n">
+      <c r="N5" s="4" t="n">
         <v>20611</v>
       </c>
-      <c r="O5" s="5" t="n">
+      <c r="O5" s="6" t="n">
         <v>3764361</v>
       </c>
       <c r="P5" s="1" t="n">
@@ -1160,6 +1179,256 @@
       </c>
       <c r="AO5" s="1" t="n">
         <v>81.82</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>20609</v>
+      </c>
+      <c r="O6" s="7" t="n">
+        <v>3770520</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>144623</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="2" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z6" s="2" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" s="1" t="n">
+        <v>18.18</v>
+      </c>
+      <c r="AC6" s="1" t="n">
+        <v>144647</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ6" s="2" t="n">
+        <v>36.36</v>
+      </c>
+      <c r="AK6" s="2" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="AL6" s="2" t="n">
+        <v>36.36</v>
+      </c>
+      <c r="AM6" s="2" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="AN6" s="2" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="AO6" s="2" t="n">
+        <v>27.27</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="N7" s="4" t="n">
+        <v>20611</v>
+      </c>
+      <c r="O7" s="7" t="n">
+        <v>3770508</v>
+      </c>
+      <c r="P7" s="1" t="n">
+        <v>144623</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X7" s="2" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z7" s="2" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" s="1" t="n">
+        <v>18.18</v>
+      </c>
+      <c r="AC7" s="1" t="n">
+        <v>144647</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ7" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="AK7" s="2" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="AL7" s="2" t="n">
+        <v>36.36</v>
+      </c>
+      <c r="AM7" s="2" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="AN7" s="2" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="AO7" s="2" t="n">
+        <v>27.27</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1182,189 +1451,191 @@
   <dimension ref="A1:AO1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S21" activeCellId="0" sqref="S21"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="43.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="4" style="1" width="12.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="17" style="2" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="12.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="1" width="12.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="31" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="4" t="s">
         <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AK1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AL1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AM1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AN1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AO1" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="4" t="n">
+      <c r="H2" s="5" t="n">
         <v>72.73</v>
       </c>
-      <c r="I2" s="4" t="n">
+      <c r="I2" s="5" t="n">
         <v>54.55</v>
       </c>
-      <c r="J2" s="4" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="K2" s="4" t="n">
+      <c r="J2" s="5" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="K2" s="5" t="n">
         <v>54.55</v>
       </c>
-      <c r="L2" s="4" t="n">
+      <c r="L2" s="5" t="n">
         <v>54.55</v>
       </c>
-      <c r="M2" s="4" t="n">
+      <c r="M2" s="5" t="n">
         <v>54.55</v>
       </c>
-      <c r="N2" s="3" t="n">
+      <c r="N2" s="4" t="n">
         <v>20609</v>
       </c>
-      <c r="O2" s="3" t="n">
+      <c r="O2" s="4" t="n">
         <v>3764377</v>
       </c>
       <c r="P2" s="1" t="n">
@@ -1447,49 +1718,49 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="3" t="n">
+      <c r="F3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="4" t="n">
         <v>54.55</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="3" t="n">
+      <c r="J3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="4" t="n">
         <v>54.55</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" s="3" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="N3" s="3" t="n">
+      <c r="L3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="4" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="N3" s="4" t="n">
         <v>20611</v>
       </c>
-      <c r="O3" s="5" t="n">
+      <c r="O3" s="6" t="n">
         <v>3764363</v>
       </c>
       <c r="P3" s="1" t="n">
@@ -1572,49 +1843,49 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="4" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="I4" s="4" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="J4" s="4" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="K4" s="4" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="L4" s="4" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="M4" s="4" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="N4" s="3" t="n">
+      <c r="B4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="N4" s="4" t="n">
         <v>20609</v>
       </c>
-      <c r="O4" s="5" t="n">
+      <c r="O4" s="6" t="n">
         <v>3764359</v>
       </c>
       <c r="P4" s="1" t="n">
@@ -1697,49 +1968,49 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="B5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="3" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="3" t="n">
+      <c r="H5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="4" t="n">
         <v>54.55</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="3" t="n">
+      <c r="L5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="4" t="n">
         <v>63.64</v>
       </c>
-      <c r="N5" s="3" t="n">
+      <c r="N5" s="4" t="n">
         <v>20611</v>
       </c>
-      <c r="O5" s="5" t="n">
+      <c r="O5" s="6" t="n">
         <v>3764361</v>
       </c>
       <c r="P5" s="1" t="n">
@@ -1819,6 +2090,256 @@
       </c>
       <c r="AO5" s="1" t="n">
         <v>81.82</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>20609</v>
+      </c>
+      <c r="O6" s="7" t="n">
+        <v>3770520</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>144623</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="2" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z6" s="2" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" s="1" t="n">
+        <v>18.18</v>
+      </c>
+      <c r="AC6" s="1" t="n">
+        <v>144647</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ6" s="2" t="n">
+        <v>36.36</v>
+      </c>
+      <c r="AK6" s="2" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="AL6" s="2" t="n">
+        <v>36.36</v>
+      </c>
+      <c r="AM6" s="2" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="AN6" s="2" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="AO6" s="2" t="n">
+        <v>27.27</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="N7" s="4" t="n">
+        <v>20611</v>
+      </c>
+      <c r="O7" s="7" t="n">
+        <v>3770508</v>
+      </c>
+      <c r="P7" s="1" t="n">
+        <v>144623</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X7" s="2" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z7" s="2" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" s="1" t="n">
+        <v>18.18</v>
+      </c>
+      <c r="AC7" s="1" t="n">
+        <v>144647</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ7" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="AK7" s="2" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="AL7" s="2" t="n">
+        <v>36.36</v>
+      </c>
+      <c r="AM7" s="2" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="AN7" s="2" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="AO7" s="2" t="n">
+        <v>27.27</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Updated some input data
</commit_message>
<xml_diff>
--- a/PythonWorkingScripts_InputData/Assessment/Audiotranscript/input_audio_transcript_cefr.xlsx
+++ b/PythonWorkingScripts_InputData/Assessment/Audiotranscript/input_audio_transcript_cefr.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="58">
   <si>
     <t xml:space="preserve">Test Cases</t>
   </si>
@@ -315,16 +315,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -341,10 +337,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -540,191 +532,191 @@
   <dimension ref="A1:AO1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="43.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="4" style="1" width="12.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="17" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="17" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="12.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="1" width="12.51"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="31" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="31" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AL1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AM1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AN1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AO1" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="5" t="n">
+      <c r="C2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="4" t="n">
         <v>72.73</v>
       </c>
-      <c r="I2" s="5" t="n">
-        <v>54.55</v>
-      </c>
-      <c r="J2" s="5" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="K2" s="5" t="n">
-        <v>54.55</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>54.55</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <v>54.55</v>
-      </c>
-      <c r="N2" s="4" t="n">
+      <c r="I2" s="4" t="n">
+        <v>54.55</v>
+      </c>
+      <c r="J2" s="4" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="K2" s="4" t="n">
+        <v>54.55</v>
+      </c>
+      <c r="L2" s="4" t="n">
+        <v>54.55</v>
+      </c>
+      <c r="M2" s="4" t="n">
+        <v>54.55</v>
+      </c>
+      <c r="N2" s="3" t="n">
         <v>20609</v>
       </c>
-      <c r="O2" s="4" t="n">
+      <c r="O2" s="3" t="n">
         <v>3764377</v>
       </c>
       <c r="P2" s="1" t="n">
@@ -807,49 +799,49 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="4" t="n">
-        <v>54.55</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="4" t="n">
-        <v>54.55</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" s="4" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="N3" s="4" t="n">
+      <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>54.55</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>54.55</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="N3" s="3" t="n">
         <v>20611</v>
       </c>
-      <c r="O3" s="6" t="n">
+      <c r="O3" s="5" t="n">
         <v>3764363</v>
       </c>
       <c r="P3" s="1" t="n">
@@ -932,49 +924,49 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="I4" s="5" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="J4" s="5" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="L4" s="5" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="M4" s="5" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="N4" s="4" t="n">
+      <c r="B4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="K4" s="4" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="L4" s="4" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="M4" s="4" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="N4" s="3" t="n">
         <v>20609</v>
       </c>
-      <c r="O4" s="6" t="n">
+      <c r="O4" s="5" t="n">
         <v>3764359</v>
       </c>
       <c r="P4" s="1" t="n">
@@ -1057,49 +1049,49 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="B5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="4" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="4" t="n">
-        <v>54.55</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="4" t="n">
+      <c r="H5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <v>54.55</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="3" t="n">
         <v>63.64</v>
       </c>
-      <c r="N5" s="4" t="n">
+      <c r="N5" s="3" t="n">
         <v>20611</v>
       </c>
-      <c r="O5" s="6" t="n">
+      <c r="O5" s="5" t="n">
         <v>3764361</v>
       </c>
       <c r="P5" s="1" t="n">
@@ -1182,254 +1174,11 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="L6" s="1" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="M6" s="1" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="N6" s="1" t="n">
-        <v>20609</v>
-      </c>
-      <c r="O6" s="7" t="n">
-        <v>3770520</v>
-      </c>
-      <c r="P6" s="1" t="n">
-        <v>144623</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="X6" s="2" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z6" s="2" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="AA6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB6" s="1" t="n">
-        <v>18.18</v>
-      </c>
-      <c r="AC6" s="1" t="n">
-        <v>144647</v>
-      </c>
-      <c r="AD6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AJ6" s="2" t="n">
-        <v>36.36</v>
-      </c>
-      <c r="AK6" s="2" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="AL6" s="2" t="n">
-        <v>36.36</v>
-      </c>
-      <c r="AM6" s="2" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="AN6" s="2" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="AO6" s="2" t="n">
-        <v>27.27</v>
-      </c>
+      <c r="O6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" s="1" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M7" s="1" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="N7" s="4" t="n">
-        <v>20611</v>
-      </c>
-      <c r="O7" s="7" t="n">
-        <v>3770508</v>
-      </c>
-      <c r="P7" s="1" t="n">
-        <v>144623</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="X7" s="2" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z7" s="2" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB7" s="1" t="n">
-        <v>18.18</v>
-      </c>
-      <c r="AC7" s="1" t="n">
-        <v>144647</v>
-      </c>
-      <c r="AD7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AJ7" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="AK7" s="2" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="AL7" s="2" t="n">
-        <v>36.36</v>
-      </c>
-      <c r="AM7" s="2" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="AN7" s="2" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="AO7" s="2" t="n">
-        <v>27.27</v>
-      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="5"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1448,194 +1197,194 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AO1048576"/>
+  <dimension ref="A1:AO7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="43.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="4" style="1" width="12.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="17" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="17" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="12.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="1" width="12.51"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="31" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="31" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AL1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AM1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AN1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AO1" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="5" t="n">
+      <c r="C2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="4" t="n">
         <v>72.73</v>
       </c>
-      <c r="I2" s="5" t="n">
-        <v>54.55</v>
-      </c>
-      <c r="J2" s="5" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="K2" s="5" t="n">
-        <v>54.55</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>54.55</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <v>54.55</v>
-      </c>
-      <c r="N2" s="4" t="n">
+      <c r="I2" s="4" t="n">
+        <v>54.55</v>
+      </c>
+      <c r="J2" s="4" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="K2" s="4" t="n">
+        <v>54.55</v>
+      </c>
+      <c r="L2" s="4" t="n">
+        <v>54.55</v>
+      </c>
+      <c r="M2" s="4" t="n">
+        <v>54.55</v>
+      </c>
+      <c r="N2" s="3" t="n">
         <v>20609</v>
       </c>
-      <c r="O2" s="4" t="n">
+      <c r="O2" s="3" t="n">
         <v>3764377</v>
       </c>
       <c r="P2" s="1" t="n">
@@ -1718,49 +1467,49 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="4" t="n">
-        <v>54.55</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="4" t="n">
-        <v>54.55</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" s="4" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="N3" s="4" t="n">
+      <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>54.55</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>54.55</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="N3" s="3" t="n">
         <v>20611</v>
       </c>
-      <c r="O3" s="6" t="n">
+      <c r="O3" s="5" t="n">
         <v>3764363</v>
       </c>
       <c r="P3" s="1" t="n">
@@ -1843,49 +1592,49 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="I4" s="5" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="J4" s="5" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="L4" s="5" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="M4" s="5" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="N4" s="4" t="n">
+      <c r="B4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="K4" s="4" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="L4" s="4" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="M4" s="4" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="N4" s="3" t="n">
         <v>20609</v>
       </c>
-      <c r="O4" s="6" t="n">
+      <c r="O4" s="5" t="n">
         <v>3764359</v>
       </c>
       <c r="P4" s="1" t="n">
@@ -1968,49 +1717,49 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="B5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="4" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="4" t="n">
-        <v>54.55</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="4" t="n">
+      <c r="H5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <v>54.55</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="3" t="n">
         <v>63.64</v>
       </c>
-      <c r="N5" s="4" t="n">
+      <c r="N5" s="3" t="n">
         <v>20611</v>
       </c>
-      <c r="O5" s="6" t="n">
+      <c r="O5" s="5" t="n">
         <v>3764361</v>
       </c>
       <c r="P5" s="1" t="n">
@@ -2135,43 +1884,43 @@
       <c r="N6" s="1" t="n">
         <v>20609</v>
       </c>
-      <c r="O6" s="7" t="n">
+      <c r="O6" s="5" t="n">
         <v>3770520</v>
       </c>
       <c r="P6" s="1" t="n">
         <v>144623</v>
       </c>
-      <c r="Q6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="V6" s="2" t="s">
+      <c r="Q6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="W6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="X6" s="2" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z6" s="2" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="AA6" s="2" t="s">
+      <c r="W6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z6" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="AA6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="AB6" s="1" t="n">
@@ -2183,37 +1932,37 @@
       <c r="AD6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AE6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF6" s="2" t="s">
+      <c r="AE6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AG6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI6" s="2" t="s">
+      <c r="AG6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AJ6" s="2" t="n">
+      <c r="AJ6" s="1" t="n">
         <v>36.36</v>
       </c>
-      <c r="AK6" s="2" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="AL6" s="2" t="n">
+      <c r="AK6" s="1" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="AL6" s="1" t="n">
         <v>36.36</v>
       </c>
-      <c r="AM6" s="2" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="AN6" s="2" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="AO6" s="2" t="n">
+      <c r="AM6" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="AN6" s="1" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="AO6" s="1" t="n">
         <v>27.27</v>
       </c>
     </row>
@@ -2257,46 +2006,46 @@
       <c r="M7" s="1" t="n">
         <v>9.09</v>
       </c>
-      <c r="N7" s="4" t="n">
+      <c r="N7" s="3" t="n">
         <v>20611</v>
       </c>
-      <c r="O7" s="7" t="n">
+      <c r="O7" s="5" t="n">
         <v>3770508</v>
       </c>
       <c r="P7" s="1" t="n">
         <v>144623</v>
       </c>
-      <c r="Q7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="V7" s="2" t="s">
+      <c r="Q7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="W7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="X7" s="2" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z7" s="2" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="AA7" s="2" t="s">
+      <c r="W7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X7" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z7" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="AA7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="AB7" s="1" t="n">
@@ -2308,41 +2057,40 @@
       <c r="AD7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AE7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF7" s="2" t="s">
+      <c r="AE7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AG7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI7" s="2" t="s">
+      <c r="AG7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AJ7" s="2" t="n">
+      <c r="AJ7" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="AK7" s="2" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="AL7" s="2" t="n">
+      <c r="AK7" s="1" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="AL7" s="1" t="n">
         <v>36.36</v>
       </c>
-      <c r="AM7" s="2" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="AN7" s="2" t="n">
-        <v>45.45</v>
-      </c>
-      <c r="AO7" s="2" t="n">
+      <c r="AM7" s="1" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="AN7" s="1" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="AO7" s="1" t="n">
         <v>27.27</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>